<commit_message>
new verison with amr updates
</commit_message>
<xml_diff>
--- a/Monitor and Control/F_RTM.xlsx
+++ b/Monitor and Control/F_RTM.xlsx
@@ -1,20 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aml\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hager\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C352B2-39E0-4EFE-A9A3-4A694C66FD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -34,23 +45,6 @@
 F_REQ_U_sig_3.2.3</t>
   </si>
   <si>
-    <t xml:space="preserve">
-F_REQ_U_sel_3.5.1
-F_REQ_U_sel_3.5.2
-F_REQ_U_meal_3.6.1
-F_REQ_U_meal_3.6.2
-F_REQ_U_meal_3.6.3
-F_REQ_U_conf_3.7.1
-F_REQ_U_conf_3.7.2
-F_REQ_U_conf_3.7.3
-F_REQ_U_conf_3.7.4
-</t>
-  </si>
-  <si>
-    <t>F_REQ_A_AddAdmin_3.21.1
-F_REQ_A_AddAdmin_3.21.2</t>
-  </si>
-  <si>
     <t>F_Cust_Req_001</t>
   </si>
   <si>
@@ -87,75 +81,74 @@
     <t>F_Cust_Req_011</t>
   </si>
   <si>
-    <t>F_REQ_U_SelOffer_3.9.1
-F_REQ_U_SelOffer_3.9.2
-F_REQ_U_SelOffer_3.9.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-F_REQ_U_offer_3.8.1
-F_REQ_U_offer_3.8.2</t>
-  </si>
-  <si>
-    <t>F_REQ_U_Reg_3.1.1
+    <t xml:space="preserve">F_REQ_U_Reg_3.1.1
 F_REQ_U_Reg_3.1.2
 F_REQ_U_sig_3.2.1
 F_REQ_U_sig_3.2.2
 F_REQ_U_sig_3.2.3
-F_REQ_U_Upd_3.3.1
-F_REQ_U_Upd_3.3.2
-F_REQ_U_Upd_3.3.3
-F_REQ_U_sear_3.10.1
-F_REQ_U_sear_3.10.2</t>
+</t>
   </si>
   <si>
     <t xml:space="preserve">
-F_REQ_U_sear_3.4.1
-F_REQ_U_sear_3.4.2
+F_REQ_U_sear_3.3.1
+F_REQ_U_sear_3.3.2
 </t>
   </si>
   <si>
-    <t>F_REQ_A_AddUser_3.10.1
-F_REQ_A_AddUser_3.10.2
-F_REQ_A_DeleteUser_3.11.1
-F_REQ_A_DeleteUser_3.11.2
-F_REQ_A_UpdateUser_3.12.1
-F_REQ_A_UpdateUser_3.12.2
-F_REQ_A_UpdateUser_3.12.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">
-F_REQ_A_AddRest_3.13.1
-F_REQ_A_AddRest_3.13.2
-F_REQ_A_DeleteRest_3.14.1
-F_REQ_A_DeleteRest_3.14.2
-F_REQ_A_UpdateRest_3.15.1
-F_REQ_A_UpdateRest_3.15.2
-F_REQ_A_UpdateRest_3.15.3
-F_REQ_A_UpdateRest_3.15.4</t>
-  </si>
-  <si>
-    <t>F_REQ_A_AddMenu_3.16.1
-F_REQ_A_AddMenu_3.16.2
-F_REQ_A_AddMenu_3.16.3
-F_REQ_A_DeleteMenu_3.17.1
-F_REQ_A_DeleteMenu_3.17.2</t>
-  </si>
-  <si>
-    <t>F_REQ_A_AddOffer_3.18.1
-F_REQ_A_AddOffer_3.18.2
-F_REQ_A_AddOffer_3.18.3
-F_REQ_A_DeleteOffer_3.19.1
-F_REQ_A_DeleteOffer_3.19.2
-F_REQ_A_UpdateOffer_3.20.1
-F_REQ_A_UpdateOffer_3.20.2
-F_REQ_A_UpdateOffer_3.20.3</t>
+F_REQ_U_sel_3.4.1
+F_REQ_U_sel_3.4.2
+F_REQ_U_meal_3.5.1
+F_REQ_U_meal_3.5.2
+F_REQ_U_meal_3.5.3
+F_REQ_U_conf_3.6.1
+F_REQ_U_conf_3.6.2
+F_REQ_U_conf_3.6.3
+F_REQ_U_conf_3.6.4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+F_REQ_U_offer_3.7.1
+F_REQ_U_offer_3.7.2</t>
+  </si>
+  <si>
+    <t>F_REQ_U_SelOffer_3.8.1
+F_REQ_U_SelOffer_3.8.2
+F_REQ_U_SelOffer_3.8.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_REQ_A_AddUser_3.9.1
+F_REQ_A_AddUser_3.9.2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+F_REQ_A_AddRest_3.10.1
+F_REQ_A_AddRest_3.10.2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_REQ_A_AddMenu_3.11.1
+F_REQ_A_AddMenu_3.11.2
+F_REQ_A_AddMenu_3.11.3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_REQ_A_AddOffer_3.12.1
+F_REQ_A_AddOffer_3.12.2
+F_REQ_A_AddOffer_3.12.3
+</t>
+  </si>
+  <si>
+    <t>F_REQ_A_AddAdmin_3.13.1
+F_REQ_A_AddAdmin_3.13.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -271,7 +264,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -320,15 +312,12 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -337,6 +326,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,31 +553,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.88671875" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" style="8" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="30" t="s">
+      <c r="A1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1"/>
@@ -604,9 +605,9 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="10"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -631,14 +632,14 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" ht="270" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="14"/>
+    <row r="3" spans="1:26" s="27" customFormat="1" ht="211.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="13"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -663,14 +664,14 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="16" t="s">
+    <row r="4" spans="1:26" s="27" customFormat="1" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -695,14 +696,14 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
     </row>
-    <row r="5" spans="1:26" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="14"/>
+    <row r="5" spans="1:26" s="27" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="13"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -727,14 +728,14 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" ht="276" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="17"/>
+    <row r="6" spans="1:26" s="27" customFormat="1" ht="276" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="16"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -745,7 +746,10 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="N6" s="4">
+        <f>+R6</f>
+        <v>0</v>
+      </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
@@ -759,14 +763,14 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:26" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="13" t="s">
+    <row r="7" spans="1:26" s="27" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -791,14 +795,14 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="17"/>
+    <row r="8" spans="1:26" s="27" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="16"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -823,14 +827,14 @@
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
     </row>
-    <row r="9" spans="1:26" ht="179.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="14"/>
+    <row r="9" spans="1:26" s="27" customFormat="1" ht="226.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="13"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -855,114 +859,114 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="220.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:26" s="27" customFormat="1" ht="112.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="28"/>
+    </row>
+    <row r="11" spans="1:26" s="27" customFormat="1" ht="159.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" s="27" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="23"/>
-    </row>
-    <row r="11" spans="1:26" ht="124.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="B12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="30"/>
+    </row>
+    <row r="13" spans="1:26" s="27" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-    </row>
-    <row r="12" spans="1:26" ht="207" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="26" t="s">
+      <c r="B13" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-    </row>
-    <row r="13" spans="1:26" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="5"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -990,7 +994,7 @@
     </row>
     <row r="17" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="8"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1018,7 +1022,7 @@
     </row>
     <row r="19" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="8"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1046,7 +1050,7 @@
     </row>
     <row r="21" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="8"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>

</xml_diff>

<commit_message>
Update the RTM with the Sequence diagram
</commit_message>
<xml_diff>
--- a/Monitor and Control/F_RTM.xlsx
+++ b/Monitor and Control/F_RTM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hager\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hager\ITI\Quality\New folder\QA_Foodies\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C352B2-39E0-4EFE-A9A3-4A694C66FD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D024F28-01DB-4618-B173-D0F6E46B4839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">SRS_Requiement </t>
   </si>
@@ -118,11 +118,6 @@
 F_REQ_U_SelOffer_3.8.3</t>
   </si>
   <si>
-    <t xml:space="preserve">F_REQ_A_AddUser_3.9.1
-F_REQ_A_AddUser_3.9.2
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 F_REQ_A_AddRest_3.10.1
 F_REQ_A_AddRest_3.10.2
@@ -143,17 +138,61 @@
   <si>
     <t>F_REQ_A_AddAdmin_3.13.1
 F_REQ_A_AddAdmin_3.13.2</t>
+  </si>
+  <si>
+    <t>F_SQ_Reg_001
+F_SQ_SignIn _002</t>
+  </si>
+  <si>
+    <t>F_SQ_SearchRes_003</t>
+  </si>
+  <si>
+    <t>F_SQ_SelectRes_004
+F_SQ_SelectMeal_005
+F_SQ_ConfirmMeal_006</t>
+  </si>
+  <si>
+    <t>F_SQ_ViewOffers&amp;Promotions_007</t>
+  </si>
+  <si>
+    <t>F_SQ_SelectOffers&amp;Promotions_008</t>
+  </si>
+  <si>
+    <t>F_REQ_A_AddUser_3.9.1
+F_REQ_A_AddUser_3.9.2</t>
+  </si>
+  <si>
+    <t>F_SQ_AddUser_009</t>
+  </si>
+  <si>
+    <t>F_SQ_AddRes_010</t>
+  </si>
+  <si>
+    <t>F_SQ_AddMenuItem_011</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F_SQ_AddOffers_012</t>
+  </si>
+  <si>
+    <t>F_SQ_AddOffers_013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -187,6 +226,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -249,95 +295,98 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,25 +608,25 @@
   </sheetPr>
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.88671875" customWidth="1"/>
     <col min="2" max="2" width="38.88671875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1"/>
@@ -632,14 +681,16 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" s="27" customFormat="1" ht="211.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="25" customFormat="1" ht="211.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="27" t="s">
+        <v>24</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -664,14 +715,16 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" s="27" customFormat="1" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="25" customFormat="1" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="28" t="s">
+        <v>24</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -696,14 +749,16 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
     </row>
-    <row r="5" spans="1:26" s="27" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" s="25" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="13"/>
+      <c r="C5" s="13" t="s">
+        <v>25</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -728,14 +783,16 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" s="27" customFormat="1" ht="276" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:26" s="25" customFormat="1" ht="276" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -763,14 +820,16 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:26" s="27" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="25" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="13"/>
+      <c r="C7" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -795,14 +854,16 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" s="27" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:26" s="25" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -827,14 +888,16 @@
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
     </row>
-    <row r="9" spans="1:26" s="27" customFormat="1" ht="226.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:26" s="25" customFormat="1" ht="145.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="13"/>
+      <c r="B9" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>30</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -859,23 +922,27 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" s="27" customFormat="1" ht="112.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:26" s="25" customFormat="1" ht="112.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="28"/>
-    </row>
-    <row r="11" spans="1:26" s="27" customFormat="1" ht="159.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="25" customFormat="1" ht="159.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="13"/>
+        <v>21</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -900,46 +967,50 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" s="27" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+    <row r="12" spans="1:26" s="25" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="26"/>
+    </row>
+    <row r="13" spans="1:26" s="25" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
-      <c r="Y12" s="30"/>
-      <c r="Z12" s="30"/>
-    </row>
-    <row r="13" spans="1:26" s="27" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="13"/>
+      <c r="C13" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1078,5 +1149,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Version Of RTM
</commit_message>
<xml_diff>
--- a/Monitor and Control/F_RTM.xlsx
+++ b/Monitor and Control/F_RTM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hager\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Desktop\QA_Foodies\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8180398C-7C0C-43A0-9DB2-71AC6F0E5842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD26616-A0C2-4C98-BAE7-E6D4C7BB4D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="197">
   <si>
     <t xml:space="preserve">F_Customer_Requirment </t>
   </si>
@@ -403,9 +403,6 @@
     <t>TC_F_AddResturant_Admin_017</t>
   </si>
   <si>
-    <t>Bug_F_AddRestaurant_Admin_007</t>
-  </si>
-  <si>
     <t>F_Cust_Req_008</t>
   </si>
   <si>
@@ -611,13 +608,22 @@
   </si>
   <si>
     <t>F_AdminAddOffer_Back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Bug_F_AddRestaurant_Admin_007</t>
+  </si>
+  <si>
+    <t>TC_F_AddResturant_Admin_018</t>
+  </si>
+  <si>
+    <t>Bug_F_AddResturant_Admin_009</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -654,6 +660,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -853,9 +865,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -864,30 +873,57 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -897,43 +933,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1218,19 +1230,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45" style="14" customWidth="1"/>
-    <col min="2" max="2" width="44.88671875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="43.88671875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="39.44140625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="53.44140625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="52.21875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="47.44140625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="45" style="13" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="43.88671875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="39.44140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="53.44140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="58.88671875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="51.109375" style="13" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
@@ -1277,1156 +1289,1156 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="F3" s="14" t="s">
+      <c r="A3" s="33"/>
+      <c r="F3" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="33"/>
+      <c r="B4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="F5" s="14" t="s">
+      <c r="A5" s="33"/>
+      <c r="F5" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="33"/>
+      <c r="B6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="F7" s="14" t="s">
+      <c r="A7" s="33"/>
+      <c r="F7" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="33"/>
+      <c r="B8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="F9" s="14" t="s">
+      <c r="A9" s="33"/>
+      <c r="F9" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="33"/>
+      <c r="B10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="F11" s="14" t="s">
+      <c r="A11" s="33"/>
+      <c r="F11" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="33"/>
+      <c r="B12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="F13" s="14" t="s">
+      <c r="A13" s="33"/>
+      <c r="F13" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="F14" s="14" t="s">
+      <c r="A14" s="33"/>
+      <c r="F14" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="F15" s="14" t="s">
+      <c r="A15" s="33"/>
+      <c r="F15" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="F16" s="14" t="s">
+      <c r="A16" s="33"/>
+      <c r="F16" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="F17" s="14" t="s">
+      <c r="A17" s="33"/>
+      <c r="F17" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-      <c r="F18" s="14" t="s">
+      <c r="A18" s="33"/>
+      <c r="F18" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="F19" s="14" t="s">
+      <c r="A19" s="33"/>
+      <c r="F19" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="F20" s="14" t="s">
+      <c r="A20" s="33"/>
+      <c r="F20" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="F21" s="14" t="s">
+      <c r="A21" s="33"/>
+      <c r="F21" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
-      <c r="F22" s="14" t="s">
+      <c r="A22" s="33"/>
+      <c r="F22" s="13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="F23" s="14" t="s">
+      <c r="A23" s="33"/>
+      <c r="F23" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
-      <c r="F24" s="14" t="s">
+      <c r="A24" s="33"/>
+      <c r="F24" s="13" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
-      <c r="F25" s="14" t="s">
+      <c r="A25" s="33"/>
+      <c r="F25" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
-      <c r="F26" s="14" t="s">
+      <c r="A26" s="33"/>
+      <c r="F26" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="F27" s="14" t="s">
+      <c r="A27" s="33"/>
+      <c r="F27" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="F28" s="14" t="s">
+      <c r="A28" s="33"/>
+      <c r="F28" s="13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
-      <c r="F29" s="14" t="s">
+      <c r="A29" s="33"/>
+      <c r="F29" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="F30" s="14" t="s">
+      <c r="A30" s="33"/>
+      <c r="F30" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="F31" s="14" t="s">
+      <c r="A31" s="33"/>
+      <c r="F31" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14" t="s">
+      <c r="A32" s="33"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G32" s="16"/>
+      <c r="G32" s="15"/>
     </row>
     <row r="33" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
     </row>
     <row r="34" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19" t="s">
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G34" s="20"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19" t="s">
+      <c r="A35" s="31"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="19"/>
+      <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="21"/>
-      <c r="B36" s="19" t="s">
+      <c r="A36" s="31"/>
+      <c r="B36" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="19"/>
+      <c r="G36" s="17"/>
     </row>
     <row r="37" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="21"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19" t="s">
+      <c r="A37" s="31"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G37" s="19"/>
+      <c r="G37" s="17"/>
     </row>
     <row r="38" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="21"/>
-      <c r="B38" s="19" t="s">
+      <c r="A38" s="31"/>
+      <c r="B38" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="19"/>
+      <c r="G38" s="17"/>
     </row>
     <row r="39" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="21"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19" t="s">
+      <c r="A39" s="31"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="19"/>
+      <c r="G39" s="17"/>
     </row>
     <row r="40" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
-      <c r="B40" s="19" t="s">
+      <c r="A40" s="31"/>
+      <c r="B40" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19" t="s">
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G40" s="19"/>
+      <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="21"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19" t="s">
+      <c r="A41" s="31"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G41" s="19"/>
+      <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="21"/>
-      <c r="B42" s="19" t="s">
+      <c r="A42" s="31"/>
+      <c r="B42" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="21"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19" t="s">
+      <c r="A43" s="31"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G43" s="19"/>
+      <c r="G43" s="17"/>
     </row>
     <row r="44" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="21"/>
-      <c r="B44" s="19" t="s">
+      <c r="A44" s="31"/>
+      <c r="B44" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19" t="s">
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G44" s="19"/>
+      <c r="G44" s="17"/>
     </row>
     <row r="45" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="21"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19" t="s">
+      <c r="A45" s="31"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G45" s="19"/>
+      <c r="G45" s="17"/>
     </row>
     <row r="46" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="21"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19" t="s">
+      <c r="A46" s="31"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G46" s="19"/>
+      <c r="G46" s="17"/>
     </row>
     <row r="47" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="21"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19" t="s">
+      <c r="A47" s="31"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G47" s="19"/>
+      <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="21"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19" t="s">
+      <c r="A48" s="31"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G48" s="19"/>
+      <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="21"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19" t="s">
+      <c r="A49" s="31"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G49" s="19"/>
+      <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="21"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19" t="s">
+      <c r="A50" s="31"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G50" s="19"/>
+      <c r="G50" s="17"/>
     </row>
     <row r="51" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="21"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19" t="s">
+      <c r="A51" s="31"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G51" s="19"/>
+      <c r="G51" s="17"/>
     </row>
     <row r="52" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="21"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19" t="s">
+      <c r="A52" s="31"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G52" s="19"/>
+      <c r="G52" s="17"/>
     </row>
     <row r="53" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="21"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19" t="s">
+      <c r="A53" s="31"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G53" s="19"/>
+      <c r="G53" s="17"/>
     </row>
     <row r="54" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="21"/>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19" t="s">
+      <c r="A54" s="31"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G54" s="19"/>
+      <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="21"/>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19" t="s">
+      <c r="A55" s="31"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G55" s="19"/>
+      <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="21"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19" t="s">
+      <c r="A56" s="31"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G56" s="19"/>
+      <c r="G56" s="17"/>
     </row>
     <row r="57" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="21"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19" t="s">
+      <c r="A57" s="31"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G57" s="19"/>
+      <c r="G57" s="17"/>
     </row>
     <row r="58" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="21"/>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19" t="s">
+      <c r="A58" s="31"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G58" s="19"/>
+      <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="21"/>
-      <c r="B59" s="19"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19" t="s">
+      <c r="A59" s="31"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="G59" s="19"/>
+      <c r="G59" s="17"/>
     </row>
     <row r="60" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="21"/>
-      <c r="B60" s="19"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19" t="s">
+      <c r="A60" s="31"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G60" s="19"/>
+      <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="21"/>
-      <c r="B61" s="19"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19" t="s">
+      <c r="A61" s="31"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G61" s="19"/>
+      <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="22"/>
-      <c r="B62" s="19"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="19" t="s">
+      <c r="A62" s="32"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G62" s="19"/>
+      <c r="G62" s="17"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
     </row>
     <row r="63" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="17"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
+      <c r="A63" s="16"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
     </row>
     <row r="64" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="23" t="s">
+      <c r="A64" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14" t="s">
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G64" s="14"/>
+      <c r="G64" s="13"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="24"/>
-      <c r="B65" s="14" t="s">
+      <c r="A65" s="37"/>
+      <c r="B65" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C65" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D65" s="14" t="s">
+      <c r="D65" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E65" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F65" s="14" t="s">
+      <c r="F65" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G65" s="25"/>
+      <c r="G65" s="19"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="24"/>
-      <c r="B66" s="14" t="s">
+      <c r="A66" s="37"/>
+      <c r="B66" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F66" s="14" t="s">
+      <c r="F66" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G66" s="26" t="s">
+      <c r="G66" s="34" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="24"/>
-      <c r="B67" s="14" t="s">
+      <c r="A67" s="37"/>
+      <c r="B67" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C67" s="14" t="s">
+      <c r="C67" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="D67" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E67" s="14" t="s">
+      <c r="E67" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="F67" s="14" t="s">
+      <c r="F67" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G67" s="26"/>
+      <c r="G67" s="34"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="24"/>
-      <c r="B68" s="14" t="s">
+      <c r="A68" s="37"/>
+      <c r="B68" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F68" s="14" t="s">
+      <c r="F68" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="G68" s="26"/>
+      <c r="G68" s="34"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="24"/>
-      <c r="B69" s="14" t="s">
+      <c r="A69" s="37"/>
+      <c r="B69" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C69" s="14" t="s">
+      <c r="C69" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D69" s="14" t="s">
+      <c r="D69" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E69" s="14" t="s">
+      <c r="E69" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F69" s="14" t="s">
+      <c r="F69" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G69" s="26"/>
+      <c r="G69" s="34"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="24"/>
-      <c r="B70" s="14" t="s">
+      <c r="A70" s="37"/>
+      <c r="B70" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F70" s="14" t="s">
+      <c r="F70" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="G70" s="26"/>
+      <c r="G70" s="34"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="24"/>
-      <c r="B71" s="14" t="s">
+      <c r="A71" s="37"/>
+      <c r="B71" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F71" s="14" t="s">
+      <c r="F71" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G71" s="27"/>
+      <c r="G71" s="35"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="24"/>
-      <c r="B72" s="14" t="s">
+      <c r="A72" s="37"/>
+      <c r="B72" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F72" s="14" t="s">
+      <c r="F72" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G72" s="28" t="s">
+      <c r="G72" s="36" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="24"/>
-      <c r="B73" s="14" t="s">
+      <c r="A73" s="37"/>
+      <c r="B73" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F73" s="14" t="s">
+      <c r="F73" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="G73" s="24"/>
+      <c r="G73" s="37"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="24"/>
-      <c r="F74" s="14" t="s">
+      <c r="A74" s="37"/>
+      <c r="F74" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G74" s="24"/>
+      <c r="G74" s="37"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="24"/>
-      <c r="F75" s="14" t="s">
+      <c r="A75" s="37"/>
+      <c r="F75" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G75" s="24"/>
+      <c r="G75" s="37"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="24"/>
-      <c r="F76" s="14" t="s">
+      <c r="A76" s="37"/>
+      <c r="F76" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G76" s="24"/>
+      <c r="G76" s="37"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="24"/>
-      <c r="F77" s="14" t="s">
+      <c r="A77" s="37"/>
+      <c r="F77" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G77" s="24"/>
+      <c r="G77" s="37"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" s="24"/>
-      <c r="F78" s="14" t="s">
+      <c r="A78" s="37"/>
+      <c r="F78" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G78" s="24"/>
+      <c r="G78" s="37"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" s="24"/>
-      <c r="B79" s="16"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="16"/>
-      <c r="E79" s="16"/>
-      <c r="F79" s="16" t="s">
+      <c r="A79" s="37"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="G79" s="24"/>
+      <c r="G79" s="37"/>
     </row>
     <row r="80" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="29"/>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14" t="s">
+      <c r="A80" s="40"/>
+      <c r="B80" s="13"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G80" s="30"/>
+      <c r="G80" s="38"/>
     </row>
     <row r="81" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="17"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="17"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-      <c r="G81" s="17"/>
+      <c r="A81" s="16"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="16"/>
     </row>
     <row r="82" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="18" t="s">
+      <c r="A82" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="19" t="s">
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="G82" s="19"/>
+      <c r="G82" s="17"/>
     </row>
     <row r="83" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="21"/>
-      <c r="B83" s="19" t="s">
+      <c r="A83" s="31"/>
+      <c r="B83" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C83" s="19"/>
-      <c r="D83" s="19"/>
-      <c r="E83" s="19"/>
-      <c r="F83" s="19" t="s">
+      <c r="C83" s="17"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="G83" s="19"/>
+      <c r="G83" s="17"/>
     </row>
     <row r="84" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="21"/>
-      <c r="B84" s="19"/>
-      <c r="C84" s="19" t="s">
+      <c r="A84" s="31"/>
+      <c r="B84" s="17"/>
+      <c r="C84" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D84" s="19" t="s">
+      <c r="D84" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E84" s="19" t="s">
+      <c r="E84" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="F84" s="19" t="s">
+      <c r="F84" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G84" s="19"/>
+      <c r="G84" s="17"/>
     </row>
     <row r="85" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="21"/>
-      <c r="B85" s="19" t="s">
+      <c r="A85" s="31"/>
+      <c r="B85" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C85" s="19"/>
-      <c r="D85" s="19"/>
-      <c r="E85" s="19"/>
-      <c r="F85" s="19"/>
-      <c r="G85" s="19"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="17"/>
     </row>
     <row r="86" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="22"/>
-      <c r="B86" s="19"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="19"/>
-      <c r="E86" s="19"/>
-      <c r="F86" s="19"/>
-      <c r="G86" s="31"/>
+      <c r="A86" s="32"/>
+      <c r="B86" s="17"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="20"/>
     </row>
     <row r="87" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="17"/>
-      <c r="B87" s="17"/>
-      <c r="C87" s="17"/>
-      <c r="D87" s="17"/>
-      <c r="E87" s="17"/>
-      <c r="F87" s="17"/>
-      <c r="G87" s="17"/>
+      <c r="A87" s="16"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="16"/>
+      <c r="E87" s="16"/>
+      <c r="F87" s="16"/>
+      <c r="G87" s="16"/>
     </row>
     <row r="88" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="23" t="s">
+      <c r="A88" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="B88" s="14" t="s">
+      <c r="B88" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="14"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
       <c r="H88" s="2"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="24"/>
-      <c r="F89" s="14" t="s">
+      <c r="A89" s="37"/>
+      <c r="F89" s="13" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="24"/>
-      <c r="B90" s="14" t="s">
+      <c r="A90" s="37"/>
+      <c r="B90" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C90" s="14" t="s">
+      <c r="C90" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D90" s="14" t="s">
+      <c r="D90" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E90" s="14" t="s">
+      <c r="E90" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="F90" s="14" t="s">
+      <c r="F90" s="13" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="24"/>
-      <c r="B91" s="14" t="s">
+      <c r="A91" s="37"/>
+      <c r="B91" s="13" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="92" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="32"/>
-      <c r="B92" s="14"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="14"/>
-      <c r="G92" s="14"/>
+      <c r="A92" s="41"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
     </row>
     <row r="93" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="17"/>
-      <c r="B93" s="17"/>
-      <c r="C93" s="17"/>
-      <c r="D93" s="17"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="17"/>
-      <c r="G93" s="17"/>
+      <c r="A93" s="16"/>
+      <c r="B93" s="16"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="16"/>
+      <c r="E93" s="16"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="16"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F94" s="16"/>
+      <c r="F94" s="15"/>
     </row>
     <row r="95" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="18" t="s">
+      <c r="A95" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B95" s="17"/>
+      <c r="C95" s="17"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="G95" s="23"/>
+    </row>
+    <row r="96" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="31"/>
+      <c r="B96" s="17"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="21"/>
+      <c r="F96" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="G96" s="23"/>
+    </row>
+    <row r="97" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="31"/>
+      <c r="B97" s="17"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="17"/>
+      <c r="F97" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="G97" s="17"/>
+    </row>
+    <row r="98" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="31"/>
+      <c r="B98" s="17"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="17"/>
+      <c r="F98" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G98" s="17"/>
+    </row>
+    <row r="99" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="31"/>
+      <c r="B99" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B95" s="19"/>
-      <c r="C95" s="19"/>
-      <c r="D95" s="19"/>
-      <c r="E95" s="33"/>
-      <c r="F95" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="G95" s="35"/>
-    </row>
-    <row r="96" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="21"/>
-      <c r="B96" s="19"/>
-      <c r="C96" s="19"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="33"/>
-      <c r="F96" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="G96" s="35"/>
-    </row>
-    <row r="97" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="21"/>
-      <c r="B97" s="19"/>
-      <c r="C97" s="19"/>
-      <c r="D97" s="19"/>
-      <c r="E97" s="19"/>
-      <c r="F97" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="G97" s="19"/>
-    </row>
-    <row r="98" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="21"/>
-      <c r="B98" s="19"/>
-      <c r="C98" s="19"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="19"/>
-      <c r="F98" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="G98" s="19"/>
-    </row>
-    <row r="99" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="21"/>
-      <c r="B99" s="19" t="s">
+      <c r="C99" s="17"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="17"/>
+      <c r="F99" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G99" s="17"/>
+    </row>
+    <row r="100" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="31"/>
+      <c r="B100" s="17"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
+      <c r="F100" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="G100" s="17"/>
+    </row>
+    <row r="101" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="31"/>
+      <c r="B101" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="C99" s="19"/>
-      <c r="D99" s="19"/>
-      <c r="E99" s="19"/>
-      <c r="F99" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="G99" s="19"/>
-    </row>
-    <row r="100" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="21"/>
-      <c r="B100" s="19"/>
-      <c r="C100" s="19"/>
-      <c r="D100" s="19"/>
-      <c r="E100" s="19"/>
-      <c r="F100" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="G100" s="19"/>
-    </row>
-    <row r="101" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="21"/>
-      <c r="B101" s="19" t="s">
+      <c r="C101" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C101" s="19" t="s">
+      <c r="D101" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="D101" s="19" t="s">
+      <c r="E101" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="E101" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="F101" s="19" t="s">
+      <c r="F101" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="G101" s="19"/>
+      <c r="G101" s="17"/>
     </row>
     <row r="102" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="21"/>
-      <c r="B102" s="19"/>
-      <c r="C102" s="19"/>
-      <c r="D102" s="19"/>
-      <c r="E102" s="19"/>
-      <c r="F102" s="19" t="s">
+      <c r="A102" s="31"/>
+      <c r="B102" s="17"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="G102" s="19" t="s">
-        <v>125</v>
+      <c r="G102" s="17" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="103" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="21"/>
-      <c r="B103" s="19"/>
-      <c r="C103" s="19"/>
-      <c r="D103" s="19"/>
-      <c r="E103" s="19"/>
-      <c r="F103" s="19" t="s">
+      <c r="A103" s="31"/>
+      <c r="B103" s="17"/>
+      <c r="C103" s="17"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="17"/>
+      <c r="F103" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="G103" s="19"/>
+      <c r="G103" s="17"/>
     </row>
     <row r="104" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="21"/>
-      <c r="B104" s="19"/>
-      <c r="C104" s="19"/>
-      <c r="D104" s="19"/>
-      <c r="E104" s="19"/>
-      <c r="F104" s="19" t="s">
+      <c r="A104" s="31"/>
+      <c r="B104" s="17"/>
+      <c r="C104" s="17"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="17"/>
+      <c r="F104" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="G104" s="19"/>
+      <c r="G104" s="17"/>
     </row>
     <row r="105" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="21"/>
-      <c r="B105" s="19"/>
-      <c r="C105" s="19"/>
-      <c r="D105" s="19"/>
-      <c r="E105" s="19"/>
-      <c r="F105" s="19" t="s">
+      <c r="A105" s="31"/>
+      <c r="B105" s="17"/>
+      <c r="C105" s="17"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="17"/>
+      <c r="F105" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="G105" s="19"/>
+      <c r="G105" s="17"/>
     </row>
     <row r="106" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="21"/>
-      <c r="B106" s="19"/>
-      <c r="C106" s="19"/>
-      <c r="D106" s="19"/>
-      <c r="E106" s="19"/>
-      <c r="F106" s="19" t="s">
+      <c r="A106" s="31"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="G106" s="19"/>
+      <c r="G106" s="17"/>
     </row>
     <row r="107" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="21"/>
-      <c r="B107" s="19"/>
-      <c r="C107" s="19"/>
-      <c r="D107" s="19"/>
-      <c r="E107" s="19"/>
-      <c r="F107" s="19" t="s">
+      <c r="A107" s="31"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="17"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="G107" s="19"/>
+      <c r="G107" s="17"/>
     </row>
     <row r="108" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="21"/>
-      <c r="B108" s="19"/>
-      <c r="C108" s="19"/>
-      <c r="D108" s="19"/>
-      <c r="E108" s="19"/>
-      <c r="F108" s="19" t="s">
+      <c r="A108" s="31"/>
+      <c r="B108" s="17"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="17"/>
+      <c r="F108" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="G108" s="19"/>
+      <c r="G108" s="17"/>
     </row>
     <row r="109" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="21"/>
-      <c r="B109" s="19"/>
-      <c r="C109" s="19"/>
-      <c r="D109" s="19"/>
-      <c r="E109" s="19"/>
-      <c r="F109" s="19" t="s">
+      <c r="A109" s="31"/>
+      <c r="B109" s="17"/>
+      <c r="C109" s="17"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="17"/>
+      <c r="F109" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="G109" s="19"/>
+      <c r="G109" s="17"/>
     </row>
     <row r="110" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="21"/>
-      <c r="B110" s="31"/>
-      <c r="C110" s="31"/>
-      <c r="D110" s="31"/>
-      <c r="E110" s="31"/>
-      <c r="F110" s="19" t="s">
+      <c r="A110" s="31"/>
+      <c r="B110" s="20"/>
+      <c r="C110" s="20"/>
+      <c r="D110" s="20"/>
+      <c r="E110" s="20"/>
+      <c r="F110" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="G110" s="19"/>
+      <c r="G110" s="17"/>
     </row>
     <row r="111" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="21"/>
-      <c r="B111" s="31"/>
-      <c r="C111" s="31"/>
-      <c r="D111" s="31"/>
-      <c r="E111" s="31"/>
-      <c r="F111" s="31" t="s">
+      <c r="A111" s="31"/>
+      <c r="B111" s="20"/>
+      <c r="C111" s="20"/>
+      <c r="D111" s="20"/>
+      <c r="E111" s="20"/>
+      <c r="F111" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="G111" s="36"/>
+      <c r="G111" s="24"/>
     </row>
     <row r="112" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="21"/>
-      <c r="B112" s="19"/>
-      <c r="C112" s="19"/>
-      <c r="D112" s="19"/>
-      <c r="E112" s="19"/>
-      <c r="F112" s="19" t="s">
+      <c r="A112" s="31"/>
+      <c r="B112" s="17"/>
+      <c r="C112" s="17"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="17"/>
+      <c r="F112" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="G112" s="19"/>
+      <c r="G112" s="17"/>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
@@ -2435,15 +2447,15 @@
       <c r="M112" s="3"/>
     </row>
     <row r="113" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="22"/>
-      <c r="B113" s="19"/>
-      <c r="C113" s="19"/>
-      <c r="D113" s="19"/>
-      <c r="E113" s="19"/>
-      <c r="F113" s="19" t="s">
+      <c r="A113" s="32"/>
+      <c r="B113" s="17"/>
+      <c r="C113" s="17"/>
+      <c r="D113" s="17"/>
+      <c r="E113" s="17"/>
+      <c r="F113" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="G113" s="19"/>
+      <c r="G113" s="17"/>
       <c r="H113" s="3"/>
       <c r="I113" s="9"/>
       <c r="J113" s="9"/>
@@ -2457,260 +2469,270 @@
       <c r="C114" s="17"/>
       <c r="D114" s="17"/>
       <c r="E114" s="17"/>
-      <c r="F114" s="17"/>
-      <c r="G114" s="17"/>
+      <c r="F114" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="G114" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="H114" s="3"/>
+      <c r="I114" s="9"/>
+      <c r="J114" s="9"/>
+      <c r="K114" s="9"/>
+      <c r="L114" s="9"/>
+      <c r="M114" s="9"/>
     </row>
     <row r="115" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="37"/>
-      <c r="B115" s="38"/>
-      <c r="C115" s="38"/>
-      <c r="D115" s="38"/>
-      <c r="E115" s="38"/>
-      <c r="F115" s="39"/>
-      <c r="G115" s="38"/>
+      <c r="A115" s="25"/>
+      <c r="B115" s="26"/>
+      <c r="C115" s="26"/>
+      <c r="D115" s="26"/>
+      <c r="E115" s="26"/>
+      <c r="F115" s="27"/>
+      <c r="G115" s="26"/>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A116" s="13" t="s">
+      <c r="A116" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="F116" s="28"/>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A117" s="33"/>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A118" s="33"/>
+      <c r="F118" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G118" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A119" s="33"/>
+      <c r="F119" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G119" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A120" s="33"/>
+      <c r="F120" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="G120" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A121" s="33"/>
+      <c r="F121" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G121" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A122" s="33"/>
+      <c r="F122" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G122" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A123" s="33"/>
+      <c r="F123" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="G123" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A124" s="33"/>
+      <c r="B124" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="F116" s="40"/>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A117" s="13"/>
-      <c r="G117" s="14" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A118" s="13"/>
-      <c r="F118" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="G118" s="14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A119" s="13"/>
-      <c r="F119" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="G119" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A120" s="13"/>
-      <c r="F120" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="G120" s="14" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A121" s="13"/>
-      <c r="F121" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="G121" s="14" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A122" s="13"/>
-      <c r="F122" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="G122" s="14" t="s">
+      <c r="F124" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="G124" s="13" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A123" s="13"/>
-      <c r="F123" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="G123" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A124" s="13"/>
-      <c r="B124" s="14" t="s">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A125" s="33"/>
+      <c r="F125" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A126" s="33"/>
+      <c r="B126" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="F124" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A125" s="13"/>
-      <c r="F125" s="14" t="s">
+      <c r="C126" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D126" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E126" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="F126" s="13" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A126" s="13"/>
-      <c r="B126" s="14" t="s">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A127" s="33"/>
+      <c r="F127" s="13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A128" s="33"/>
+      <c r="B128" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="C126" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="D126" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="E126" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="F126" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A127" s="13"/>
-      <c r="F127" s="14" t="s">
+      <c r="F128" s="13" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A128" s="13"/>
-      <c r="B128" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="F128" s="14" t="s">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A129" s="33"/>
+      <c r="F129" s="13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A129" s="13"/>
-      <c r="F129" s="14" t="s">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A130" s="33"/>
+      <c r="F130" s="13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A130" s="13"/>
-      <c r="F130" s="14" t="s">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A131" s="33"/>
+      <c r="F131" s="13" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A131" s="13"/>
-      <c r="F131" s="14" t="s">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A132" s="33"/>
+      <c r="F132" s="13" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A132" s="13"/>
-      <c r="F132" s="14" t="s">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A133" s="33"/>
+      <c r="F133" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A133" s="13"/>
-      <c r="F133" s="14" t="s">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A134" s="33"/>
+      <c r="F134" s="13" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A134" s="13"/>
-      <c r="F134" s="14" t="s">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A135" s="33"/>
+      <c r="F135" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A135" s="13"/>
-      <c r="F135" s="14" t="s">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136" s="33"/>
+      <c r="F136" s="13" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A136" s="13"/>
-      <c r="F136" s="14" t="s">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137" s="33"/>
+      <c r="F137" s="13" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A137" s="13"/>
-      <c r="F137" s="14" t="s">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138" s="33"/>
+      <c r="F138" s="13" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A138" s="13"/>
-      <c r="F138" s="14" t="s">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A139" s="33"/>
+      <c r="F139" s="13" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A139" s="13"/>
-      <c r="F139" s="14" t="s">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A140" s="33"/>
+      <c r="F140" s="13" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A140" s="13"/>
-      <c r="F140" s="14" t="s">
+    <row r="141" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="33"/>
+      <c r="B141" s="28"/>
+      <c r="C141" s="28"/>
+      <c r="D141" s="28"/>
+      <c r="E141" s="28"/>
+      <c r="F141" s="13" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="13"/>
-      <c r="B141" s="40"/>
-      <c r="C141" s="40"/>
-      <c r="D141" s="40"/>
-      <c r="E141" s="40"/>
-      <c r="F141" s="14" t="s">
+      <c r="G141" s="28"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A142" s="33"/>
+      <c r="F142" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="G141" s="40"/>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A142" s="13"/>
-      <c r="F142" s="14" t="s">
-        <v>156</v>
-      </c>
     </row>
     <row r="143" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="16"/>
-      <c r="B143" s="16"/>
-      <c r="C143" s="16"/>
-      <c r="D143" s="16"/>
-      <c r="E143" s="16"/>
-      <c r="F143" s="41"/>
-      <c r="G143" s="16"/>
+      <c r="A143" s="15"/>
+      <c r="B143" s="15"/>
+      <c r="C143" s="15"/>
+      <c r="D143" s="15"/>
+      <c r="E143" s="15"/>
+      <c r="F143" s="29"/>
+      <c r="G143" s="15"/>
     </row>
     <row r="144" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="17"/>
-      <c r="B144" s="17"/>
-      <c r="C144" s="17"/>
-      <c r="D144" s="17"/>
-      <c r="E144" s="17"/>
-      <c r="F144" s="17"/>
-      <c r="G144" s="17"/>
+      <c r="A144" s="16"/>
+      <c r="B144" s="16"/>
+      <c r="C144" s="16"/>
+      <c r="D144" s="16"/>
+      <c r="E144" s="16"/>
+      <c r="F144" s="16"/>
+      <c r="G144" s="16"/>
     </row>
     <row r="145" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="38"/>
-      <c r="B145" s="38"/>
-      <c r="C145" s="38"/>
-      <c r="D145" s="38"/>
-      <c r="E145" s="38"/>
-      <c r="F145" s="38"/>
-      <c r="G145" s="38"/>
+      <c r="A145" s="26"/>
+      <c r="B145" s="26"/>
+      <c r="C145" s="26"/>
+      <c r="D145" s="26"/>
+      <c r="E145" s="26"/>
+      <c r="F145" s="26"/>
+      <c r="G145" s="26"/>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A147" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="B147" s="19"/>
-      <c r="C147" s="19"/>
-      <c r="D147" s="19"/>
-      <c r="E147" s="19"/>
-      <c r="F147" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="G147" s="19"/>
+      <c r="A147" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="B147" s="17"/>
+      <c r="C147" s="17"/>
+      <c r="D147" s="17"/>
+      <c r="E147" s="17"/>
+      <c r="F147" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="G147" s="17"/>
       <c r="H147" s="3"/>
       <c r="I147" s="3"/>
       <c r="J147" s="3"/>
@@ -2722,15 +2744,15 @@
       <c r="P147" s="3"/>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A148" s="21"/>
-      <c r="B148" s="19"/>
-      <c r="C148" s="19"/>
-      <c r="D148" s="19"/>
-      <c r="E148" s="19"/>
-      <c r="F148" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="G148" s="19"/>
+      <c r="A148" s="31"/>
+      <c r="B148" s="17"/>
+      <c r="C148" s="17"/>
+      <c r="D148" s="17"/>
+      <c r="E148" s="17"/>
+      <c r="F148" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="G148" s="17"/>
       <c r="H148" s="3"/>
       <c r="I148" s="3"/>
       <c r="J148" s="3"/>
@@ -2742,17 +2764,17 @@
       <c r="P148" s="3"/>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A149" s="21"/>
-      <c r="B149" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="C149" s="19"/>
-      <c r="D149" s="19"/>
-      <c r="E149" s="19"/>
-      <c r="F149" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="G149" s="19"/>
+      <c r="A149" s="31"/>
+      <c r="B149" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C149" s="17"/>
+      <c r="D149" s="17"/>
+      <c r="E149" s="17"/>
+      <c r="F149" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G149" s="17"/>
       <c r="H149" s="3"/>
       <c r="I149" s="3"/>
       <c r="J149" s="3"/>
@@ -2764,15 +2786,15 @@
       <c r="P149" s="3"/>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A150" s="21"/>
-      <c r="B150" s="19"/>
-      <c r="C150" s="19"/>
-      <c r="D150" s="19"/>
-      <c r="E150" s="19"/>
-      <c r="F150" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="G150" s="19"/>
+      <c r="A150" s="31"/>
+      <c r="B150" s="17"/>
+      <c r="C150" s="17"/>
+      <c r="D150" s="17"/>
+      <c r="E150" s="17"/>
+      <c r="F150" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G150" s="17"/>
       <c r="H150" s="3"/>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
@@ -2784,19 +2806,19 @@
       <c r="P150" s="3"/>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A151" s="21"/>
-      <c r="B151" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="C151" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="D151" s="19"/>
-      <c r="E151" s="19"/>
-      <c r="F151" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="G151" s="19"/>
+      <c r="A151" s="31"/>
+      <c r="B151" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C151" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="D151" s="17"/>
+      <c r="E151" s="17"/>
+      <c r="F151" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G151" s="17"/>
       <c r="H151" s="3"/>
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
@@ -2808,19 +2830,19 @@
       <c r="P151" s="3"/>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A152" s="21"/>
-      <c r="B152" s="19"/>
-      <c r="C152" s="19"/>
-      <c r="D152" s="19" t="s">
+      <c r="A152" s="31"/>
+      <c r="B152" s="17"/>
+      <c r="C152" s="17"/>
+      <c r="D152" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="E152" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="E152" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="F152" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="G152" s="19"/>
+      <c r="F152" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="G152" s="17"/>
       <c r="H152" s="3"/>
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
@@ -2832,17 +2854,17 @@
       <c r="P152" s="3"/>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A153" s="21"/>
-      <c r="B153" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="C153" s="19"/>
-      <c r="D153" s="19"/>
-      <c r="E153" s="19"/>
-      <c r="F153" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="G153" s="19"/>
+      <c r="A153" s="31"/>
+      <c r="B153" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C153" s="17"/>
+      <c r="D153" s="17"/>
+      <c r="E153" s="17"/>
+      <c r="F153" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G153" s="17"/>
       <c r="H153" s="3"/>
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
@@ -2854,15 +2876,15 @@
       <c r="P153" s="3"/>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A154" s="21"/>
-      <c r="B154" s="19"/>
-      <c r="C154" s="19"/>
-      <c r="D154" s="19"/>
-      <c r="E154" s="19"/>
-      <c r="F154" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="G154" s="19"/>
+      <c r="A154" s="31"/>
+      <c r="B154" s="17"/>
+      <c r="C154" s="17"/>
+      <c r="D154" s="17"/>
+      <c r="E154" s="17"/>
+      <c r="F154" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="G154" s="17"/>
       <c r="H154" s="3"/>
       <c r="I154" s="3"/>
       <c r="J154" s="3"/>
@@ -2874,15 +2896,15 @@
       <c r="P154" s="3"/>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A155" s="21"/>
-      <c r="B155" s="19"/>
-      <c r="C155" s="19"/>
-      <c r="D155" s="19"/>
-      <c r="E155" s="19"/>
-      <c r="F155" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="G155" s="19"/>
+      <c r="A155" s="31"/>
+      <c r="B155" s="17"/>
+      <c r="C155" s="17"/>
+      <c r="D155" s="17"/>
+      <c r="E155" s="17"/>
+      <c r="F155" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="G155" s="17"/>
       <c r="H155" s="3"/>
       <c r="I155" s="3"/>
       <c r="J155" s="3"/>
@@ -2894,15 +2916,15 @@
       <c r="P155" s="3"/>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A156" s="21"/>
-      <c r="B156" s="19"/>
-      <c r="C156" s="19"/>
-      <c r="D156" s="19"/>
-      <c r="E156" s="19"/>
-      <c r="F156" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="G156" s="19"/>
+      <c r="A156" s="31"/>
+      <c r="B156" s="17"/>
+      <c r="C156" s="17"/>
+      <c r="D156" s="17"/>
+      <c r="E156" s="17"/>
+      <c r="F156" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="G156" s="17"/>
       <c r="H156" s="3"/>
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
@@ -2914,15 +2936,15 @@
       <c r="P156" s="3"/>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A157" s="21"/>
-      <c r="B157" s="19"/>
-      <c r="C157" s="19"/>
-      <c r="D157" s="19"/>
-      <c r="E157" s="19"/>
-      <c r="F157" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="G157" s="19"/>
+      <c r="A157" s="31"/>
+      <c r="B157" s="17"/>
+      <c r="C157" s="17"/>
+      <c r="D157" s="17"/>
+      <c r="E157" s="17"/>
+      <c r="F157" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="G157" s="17"/>
       <c r="H157" s="3"/>
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
@@ -2934,15 +2956,15 @@
       <c r="P157" s="3"/>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A158" s="21"/>
-      <c r="B158" s="19"/>
-      <c r="C158" s="19"/>
-      <c r="D158" s="19"/>
-      <c r="E158" s="19"/>
-      <c r="F158" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="G158" s="19"/>
+      <c r="A158" s="31"/>
+      <c r="B158" s="17"/>
+      <c r="C158" s="17"/>
+      <c r="D158" s="17"/>
+      <c r="E158" s="17"/>
+      <c r="F158" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="G158" s="17"/>
       <c r="H158" s="3"/>
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
@@ -2954,15 +2976,15 @@
       <c r="P158" s="3"/>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A159" s="21"/>
-      <c r="B159" s="19"/>
-      <c r="C159" s="19"/>
-      <c r="D159" s="19"/>
-      <c r="E159" s="19"/>
-      <c r="F159" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="G159" s="19"/>
+      <c r="A159" s="31"/>
+      <c r="B159" s="17"/>
+      <c r="C159" s="17"/>
+      <c r="D159" s="17"/>
+      <c r="E159" s="17"/>
+      <c r="F159" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="G159" s="17"/>
       <c r="H159" s="3"/>
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
@@ -2974,15 +2996,15 @@
       <c r="P159" s="3"/>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A160" s="21"/>
-      <c r="B160" s="19"/>
-      <c r="C160" s="19"/>
-      <c r="D160" s="19"/>
-      <c r="E160" s="19"/>
-      <c r="F160" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="G160" s="19"/>
+      <c r="A160" s="31"/>
+      <c r="B160" s="17"/>
+      <c r="C160" s="17"/>
+      <c r="D160" s="17"/>
+      <c r="E160" s="17"/>
+      <c r="F160" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="G160" s="17"/>
       <c r="H160" s="3"/>
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
@@ -2994,15 +3016,15 @@
       <c r="P160" s="3"/>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A161" s="22"/>
-      <c r="B161" s="19"/>
-      <c r="C161" s="19"/>
-      <c r="D161" s="19"/>
-      <c r="E161" s="19"/>
-      <c r="F161" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="G161" s="19"/>
+      <c r="A161" s="32"/>
+      <c r="B161" s="17"/>
+      <c r="C161" s="17"/>
+      <c r="D161" s="17"/>
+      <c r="E161" s="17"/>
+      <c r="F161" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="G161" s="17"/>
       <c r="H161" s="3"/>
       <c r="I161" s="3"/>
       <c r="J161" s="3"/>
@@ -3015,6 +3037,8 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A32"/>
+    <mergeCell ref="A34:A62"/>
     <mergeCell ref="A95:A113"/>
     <mergeCell ref="A116:A142"/>
     <mergeCell ref="A147:A161"/>
@@ -3023,9 +3047,8 @@
     <mergeCell ref="A64:A80"/>
     <mergeCell ref="A82:A86"/>
     <mergeCell ref="A88:A92"/>
-    <mergeCell ref="A2:A32"/>
-    <mergeCell ref="A34:A62"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>